<commit_message>
Added peptide mapping analyses.
</commit_message>
<xml_diff>
--- a/data/SampleList.xlsx
+++ b/data/SampleList.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="751" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25280" windowHeight="15960" tabRatio="751"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="105">
   <si>
     <t>Sample #</t>
   </si>
@@ -152,7 +156,7 @@
     <t>PA14</t>
   </si>
   <si>
-    <t> </t>
+    <t/>
   </si>
   <si>
     <t>PA15</t>
@@ -303,18 +307,43 @@
   </si>
   <si>
     <t>wild10A-46-9min-rep2.fastq</t>
+  </si>
+  <si>
+    <t>PA46</t>
+  </si>
+  <si>
+    <t>PA47</t>
+  </si>
+  <si>
+    <t>PA48</t>
+  </si>
+  <si>
+    <t>PA49</t>
+  </si>
+  <si>
+    <t>PA50</t>
+  </si>
+  <si>
+    <t>PA51</t>
+  </si>
+  <si>
+    <t>PA52</t>
+  </si>
+  <si>
+    <t>PA53</t>
+  </si>
+  <si>
+    <t>PA54</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -323,23 +352,24 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="12"/>
+      <color rgb="FF3B4045"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
+      <u/>
       <sz val="12"/>
-      <color rgb="FF3B4045"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -354,7 +384,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -362,65 +392,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -479,39 +495,359 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF3B4045"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:N46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.662962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.662962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.4925925925926"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.4925925925926"/>
+    <col min="3" max="9" width="8.83203125" style="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -532,24 +868,24 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -567,25 +903,25 @@
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="0"/>
+      <c r="H2"/>
       <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3" t="n">
+      <c r="K2" s="3">
         <v>42020</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="3">
         <v>42012</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -603,25 +939,25 @@
       <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="0"/>
+      <c r="H3"/>
       <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="3">
         <v>42020</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="3">
         <v>42012</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -639,25 +975,25 @@
       <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="0"/>
+      <c r="H4"/>
       <c r="J4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="3">
         <v>42020</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="3">
         <v>42012</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -675,25 +1011,25 @@
       <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="0"/>
+      <c r="H5"/>
       <c r="J5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="3">
         <v>42020</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="3">
         <v>42012</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -711,25 +1047,25 @@
       <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="0"/>
+      <c r="H6"/>
       <c r="J6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="3">
         <v>42020</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="3">
         <v>42012</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -747,25 +1083,25 @@
       <c r="G7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="0"/>
+      <c r="H7"/>
       <c r="J7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="3">
         <v>42020</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="3">
         <v>42012</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -783,25 +1119,25 @@
       <c r="G8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="0"/>
+      <c r="H8"/>
       <c r="J8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="K8" s="3">
         <v>42020</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="3">
         <v>42012</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -819,25 +1155,25 @@
       <c r="G9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="0"/>
+      <c r="H9"/>
       <c r="J9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="3" t="n">
+      <c r="K9" s="3">
         <v>42020</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="3">
         <v>42012</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -855,25 +1191,25 @@
       <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="0"/>
+      <c r="H10"/>
       <c r="J10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="3">
         <v>42020</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="3">
         <v>42012</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -891,25 +1227,25 @@
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="0"/>
-      <c r="J11" s="0" t="s">
+      <c r="H11"/>
+      <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L11" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M11" s="0" t="s">
+      <c r="K11" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L11" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -927,25 +1263,25 @@
       <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="0"/>
-      <c r="J12" s="0" t="s">
+      <c r="H12"/>
+      <c r="J12" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L12" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M12" s="0" t="s">
+      <c r="K12" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L12" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -963,25 +1299,25 @@
       <c r="G13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="0"/>
-      <c r="J13" s="0" t="s">
+      <c r="H13"/>
+      <c r="J13" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L13" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M13" s="0" t="s">
+      <c r="K13" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L13" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -999,25 +1335,25 @@
       <c r="G14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="0"/>
-      <c r="J14" s="0" t="s">
+      <c r="H14"/>
+      <c r="J14" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L14" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M14" s="0" t="s">
+      <c r="K14" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L14" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1035,28 +1371,28 @@
       <c r="G15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="0"/>
-      <c r="J15" s="0" t="s">
+      <c r="H15"/>
+      <c r="J15" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L15" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M15" s="0" t="s">
+      <c r="K15" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L15" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M15" t="s">
         <v>5</v>
       </c>
-      <c r="N15" s="0" t="s">
+      <c r="N15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1074,25 +1410,25 @@
       <c r="G16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="0"/>
-      <c r="J16" s="0" t="s">
+      <c r="H16"/>
+      <c r="J16" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L16" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M16" s="0" t="s">
+      <c r="K16" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L16" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1110,25 +1446,25 @@
       <c r="G17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="0"/>
-      <c r="J17" s="0" t="s">
+      <c r="H17"/>
+      <c r="J17" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L17" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M17" s="0" t="s">
+      <c r="K17" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L17" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1146,25 +1482,25 @@
       <c r="G18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="0"/>
-      <c r="J18" s="0" t="s">
+      <c r="H18"/>
+      <c r="J18" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L18" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M18" s="0" t="s">
+      <c r="K18" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L18" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1182,25 +1518,25 @@
       <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="0"/>
-      <c r="J19" s="0" t="s">
+      <c r="H19"/>
+      <c r="J19" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="L19" s="4" t="n">
-        <v>42178</v>
-      </c>
-      <c r="M19" s="0" t="s">
+      <c r="K19" s="4">
+        <v>42178</v>
+      </c>
+      <c r="L19" s="4">
+        <v>42178</v>
+      </c>
+      <c r="M19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1218,25 +1554,25 @@
       <c r="G20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="0"/>
+      <c r="H20"/>
       <c r="J20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K20" s="3" t="n">
+      <c r="K20" s="3">
         <v>42310</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="L20" s="3">
         <v>42178</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1254,25 +1590,25 @@
       <c r="G21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="0"/>
+      <c r="H21"/>
       <c r="J21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="3" t="n">
+      <c r="K21" s="3">
         <v>42310</v>
       </c>
-      <c r="L21" s="3" t="n">
+      <c r="L21" s="3">
         <v>42178</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1290,25 +1626,25 @@
       <c r="G22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="0"/>
+      <c r="H22"/>
       <c r="J22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="3" t="n">
+      <c r="K22" s="3">
         <v>42310</v>
       </c>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="3">
         <v>42178</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1326,25 +1662,25 @@
       <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="0"/>
+      <c r="H23"/>
       <c r="J23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K23" s="3" t="n">
+      <c r="K23" s="3">
         <v>42310</v>
       </c>
-      <c r="L23" s="3" t="n">
+      <c r="L23" s="3">
         <v>42178</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1362,25 +1698,25 @@
       <c r="G24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="0"/>
+      <c r="H24"/>
       <c r="J24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="3" t="n">
+      <c r="K24" s="3">
         <v>42310</v>
       </c>
-      <c r="L24" s="3" t="n">
+      <c r="L24" s="3">
         <v>42178</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1398,25 +1734,25 @@
       <c r="G25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="0"/>
+      <c r="H25"/>
       <c r="J25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="3" t="n">
+      <c r="K25" s="3">
         <v>42310</v>
       </c>
-      <c r="L25" s="3" t="n">
+      <c r="L25" s="3">
         <v>42178</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1434,25 +1770,25 @@
       <c r="G26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="0"/>
+      <c r="H26"/>
       <c r="J26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K26" s="3" t="n">
+      <c r="K26" s="3">
         <v>42310</v>
       </c>
-      <c r="L26" s="3" t="n">
+      <c r="L26" s="3">
         <v>42178</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1470,25 +1806,25 @@
       <c r="G27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="0"/>
+      <c r="H27"/>
       <c r="J27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="3" t="n">
+      <c r="K27" s="3">
         <v>42310</v>
       </c>
-      <c r="L27" s="3" t="n">
+      <c r="L27" s="3">
         <v>42178</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1506,25 +1842,25 @@
       <c r="G28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="0"/>
+      <c r="H28"/>
       <c r="J28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="3" t="n">
+      <c r="K28" s="3">
         <v>42310</v>
       </c>
-      <c r="L28" s="3" t="n">
+      <c r="L28" s="3">
         <v>42178</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1545,24 +1881,24 @@
       <c r="H29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" t="s">
         <v>19</v>
       </c>
-      <c r="K29" s="4" t="n">
+      <c r="K29" s="4">
         <v>42276</v>
       </c>
-      <c r="L29" s="4" t="n">
+      <c r="L29" s="4">
         <v>42178</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1583,24 +1919,24 @@
       <c r="H30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" t="s">
         <v>22</v>
       </c>
-      <c r="K30" s="4" t="n">
+      <c r="K30" s="4">
         <v>42276</v>
       </c>
-      <c r="L30" s="4" t="n">
+      <c r="L30" s="4">
         <v>42178</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1621,24 +1957,24 @@
       <c r="H31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" t="s">
         <v>25</v>
       </c>
-      <c r="K31" s="4" t="n">
+      <c r="K31" s="4">
         <v>42276</v>
       </c>
-      <c r="L31" s="4" t="n">
+      <c r="L31" s="4">
         <v>42178</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1659,24 +1995,24 @@
       <c r="H32" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="J32" t="s">
         <v>28</v>
       </c>
-      <c r="K32" s="4" t="n">
+      <c r="K32" s="4">
         <v>42276</v>
       </c>
-      <c r="L32" s="4" t="n">
+      <c r="L32" s="4">
         <v>42178</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:13">
+      <c r="A33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1697,24 +2033,24 @@
       <c r="H33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="J33" t="s">
         <v>30</v>
       </c>
-      <c r="K33" s="4" t="n">
+      <c r="K33" s="4">
         <v>42276</v>
       </c>
-      <c r="L33" s="4" t="n">
+      <c r="L33" s="4">
         <v>42178</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1735,24 +2071,24 @@
       <c r="H34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="J34" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="4" t="n">
+      <c r="K34" s="4">
         <v>42276</v>
       </c>
-      <c r="L34" s="4" t="n">
+      <c r="L34" s="4">
         <v>42178</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:13">
+      <c r="A35" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1773,24 +2109,24 @@
       <c r="H35" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" t="s">
         <v>35</v>
       </c>
-      <c r="K35" s="4" t="n">
+      <c r="K35" s="4">
         <v>42276</v>
       </c>
-      <c r="L35" s="4" t="n">
+      <c r="L35" s="4">
         <v>42178</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:13">
+      <c r="A36" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1811,24 +2147,24 @@
       <c r="H36" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="J36" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="4" t="n">
+      <c r="K36" s="4">
         <v>42276</v>
       </c>
-      <c r="L36" s="4" t="n">
+      <c r="L36" s="4">
         <v>42178</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:13">
+      <c r="A37" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1849,24 +2185,24 @@
       <c r="H37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="J37" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="4" t="n">
+      <c r="K37" s="4">
         <v>42276</v>
       </c>
-      <c r="L37" s="4" t="n">
+      <c r="L37" s="4">
         <v>42178</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:13">
+      <c r="A38" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1887,24 +2223,24 @@
       <c r="H38" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="J38" t="s">
         <v>19</v>
       </c>
-      <c r="K38" s="4" t="n">
+      <c r="K38" s="4">
         <v>42276</v>
       </c>
-      <c r="L38" s="4" t="n">
+      <c r="L38" s="4">
         <v>42178</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:13">
+      <c r="A39" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1925,24 +2261,24 @@
       <c r="H39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="J39" t="s">
         <v>22</v>
       </c>
-      <c r="K39" s="4" t="n">
+      <c r="K39" s="4">
         <v>42276</v>
       </c>
-      <c r="L39" s="4" t="n">
+      <c r="L39" s="4">
         <v>42178</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1963,24 +2299,24 @@
       <c r="H40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="J40" t="s">
         <v>25</v>
       </c>
-      <c r="K40" s="4" t="n">
+      <c r="K40" s="4">
         <v>42276</v>
       </c>
-      <c r="L40" s="4" t="n">
+      <c r="L40" s="4">
         <v>42178</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:13">
+      <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -2001,24 +2337,24 @@
       <c r="H41" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="J41" t="s">
         <v>28</v>
       </c>
-      <c r="K41" s="4" t="n">
+      <c r="K41" s="4">
         <v>42276</v>
       </c>
-      <c r="L41" s="4" t="n">
+      <c r="L41" s="4">
         <v>42178</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -2039,24 +2375,24 @@
       <c r="H42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J42" t="s">
         <v>30</v>
       </c>
-      <c r="K42" s="4" t="n">
+      <c r="K42" s="4">
         <v>42276</v>
       </c>
-      <c r="L42" s="4" t="n">
+      <c r="L42" s="4">
         <v>42178</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -2077,24 +2413,24 @@
       <c r="H43" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J43" t="s">
         <v>32</v>
       </c>
-      <c r="K43" s="4" t="n">
+      <c r="K43" s="4">
         <v>42276</v>
       </c>
-      <c r="L43" s="4" t="n">
+      <c r="L43" s="4">
         <v>42178</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:13">
+      <c r="A44" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -2115,24 +2451,24 @@
       <c r="H44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="J44" t="s">
         <v>35</v>
       </c>
-      <c r="K44" s="4" t="n">
+      <c r="K44" s="4">
         <v>42276</v>
       </c>
-      <c r="L44" s="4" t="n">
+      <c r="L44" s="4">
         <v>42178</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:13">
+      <c r="A45" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -2153,24 +2489,24 @@
       <c r="H45" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J45" s="0" t="s">
+      <c r="J45" t="s">
         <v>37</v>
       </c>
-      <c r="K45" s="4" t="n">
+      <c r="K45" s="4">
         <v>42276</v>
       </c>
-      <c r="L45" s="4" t="n">
+      <c r="L45" s="4">
         <v>42178</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:13">
+      <c r="A46" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -2191,26 +2527,341 @@
       <c r="H46" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" t="s">
         <v>39</v>
       </c>
-      <c r="K46" s="4" t="n">
+      <c r="K46" s="4">
         <v>42276</v>
       </c>
-      <c r="L46" s="4" t="n">
+      <c r="L46" s="4">
         <v>42178</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>61</v>
       </c>
     </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L47" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L48" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" t="s">
+        <v>25</v>
+      </c>
+      <c r="K49" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L49" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L50" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" t="s">
+        <v>30</v>
+      </c>
+      <c r="K51" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L51" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L52" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" t="s">
+        <v>35</v>
+      </c>
+      <c r="K53" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L53" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" t="s">
+        <v>37</v>
+      </c>
+      <c r="K54" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L54" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" t="s">
+        <v>39</v>
+      </c>
+      <c r="K55" s="6">
+        <v>42565</v>
+      </c>
+      <c r="L55" s="6">
+        <v>42396</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>